<commit_message>
- v4 design update - Removed SQLite dependency favoring wasm result - TODO: Performance tuning pending
</commit_message>
<xml_diff>
--- a/rs/src/tests/TestFiles/basic_test.xlsx
+++ b/rs/src/tests/TestFiles/basic_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\draviavemal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E942EFB1-70A6-4A40-858D-830978E8D852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17606B1-6AE4-4585-A1ED-53244B14AA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="3345" windowWidth="34065" windowHeight="15345" activeTab="1" xr2:uid="{55A69094-CFF0-4A24-937F-3F8966A07938}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{55A69094-CFF0-4A24-937F-3F8966A07938}"/>
   </bookViews>
   <sheets>
     <sheet name="Style" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>Merge Cell</t>
   </si>
   <si>
-    <t>val 1</t>
-  </si>
-  <si>
     <t>val 2</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>Input Blue org</t>
+  </si>
+  <si>
+    <t>val 1 &amp; test</t>
   </si>
 </sst>
 </file>
@@ -508,22 +508,22 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -666,6 +666,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -673,12 +679,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -710,7 +710,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A229BDC0-03F6-4E22-BFCB-15D343301F0E}" name="Table2" displayName="Table2" ref="M8:P17" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A229BDC0-03F6-4E22-BFCB-15D343301F0E}" name="Table2" displayName="Table2" ref="M8:P17" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="M8:P17" xr:uid="{A229BDC0-03F6-4E22-BFCB-15D343301F0E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{76FE2717-F7CB-41BC-8D86-46E0E7B52331}" name="1" dataDxfId="3"/>
@@ -1145,21 +1145,21 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1174,11 +1174,12 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="6" max="8" width="11" customWidth="1"/>
@@ -1187,17 +1188,17 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
       </c>
       <c r="D1" t="str">
         <f>_xlfn.CONCAT(A1,B1,C1)</f>
-        <v>val 1val 2res</v>
+        <v>val 1 &amp; testval 2res</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1213,7 +1214,7 @@
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(A1:C1)</f>
-        <v>val 1val 2res</v>
+        <v>val 1 &amp; testval 2res</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1287,17 +1288,17 @@
         <f>SUM(A8:B8)</f>
         <v>83</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="O8" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="P8" s="34" t="s">
         <v>33</v>
-      </c>
-      <c r="P8" s="35" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1311,16 +1312,16 @@
         <f>AVERAGE(A9,B9)</f>
         <v>41.7</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="30">
         <v>2</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="30">
         <v>4</v>
       </c>
-      <c r="O9" s="32">
+      <c r="O9" s="31">
         <v>6</v>
       </c>
-      <c r="P9" s="30">
+      <c r="P9" s="29">
         <v>8</v>
       </c>
     </row>
@@ -1335,16 +1336,16 @@
         <f>AVERAGE(A10:B10)</f>
         <v>39.9</v>
       </c>
-      <c r="M10" s="28">
+      <c r="M10" s="27">
         <v>3</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="27">
         <v>6</v>
       </c>
-      <c r="O10" s="29">
+      <c r="O10" s="28">
         <v>9</v>
       </c>
-      <c r="P10" s="27">
+      <c r="P10" s="26">
         <v>12</v>
       </c>
     </row>
@@ -1359,16 +1360,16 @@
         <f>ABS(A11-B11)</f>
         <v>31.55</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="30">
         <v>4</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="30">
         <v>8</v>
       </c>
-      <c r="O11" s="32">
+      <c r="O11" s="31">
         <v>12</v>
       </c>
-      <c r="P11" s="30">
+      <c r="P11" s="29">
         <v>16</v>
       </c>
     </row>
@@ -1384,24 +1385,24 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>29</v>
       </c>
-      <c r="H12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" s="28">
+      <c r="M12" s="27">
         <v>5</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12" s="27">
         <v>10</v>
       </c>
-      <c r="O12" s="29">
+      <c r="O12" s="28">
         <v>15</v>
       </c>
-      <c r="P12" s="27">
+      <c r="P12" s="26">
         <v>20</v>
       </c>
     </row>
@@ -1421,16 +1422,16 @@
       <c r="H13">
         <v>3</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="30">
         <v>6</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="30">
         <v>12</v>
       </c>
-      <c r="O13" s="32">
+      <c r="O13" s="31">
         <v>18</v>
       </c>
-      <c r="P13" s="30">
+      <c r="P13" s="29">
         <v>24</v>
       </c>
     </row>
@@ -1450,20 +1451,20 @@
       <c r="H14">
         <v>6</v>
       </c>
-      <c r="M14" s="28">
+      <c r="M14" s="27">
         <v>7</v>
       </c>
-      <c r="N14" s="28">
+      <c r="N14" s="27">
         <v>14</v>
       </c>
-      <c r="O14" s="29">
+      <c r="O14" s="28">
         <v>21</v>
       </c>
-      <c r="P14" s="27">
+      <c r="P14" s="26">
         <v>28</v>
       </c>
-      <c r="T14" s="39" t="s">
-        <v>35</v>
+      <c r="T14" s="38" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1482,16 +1483,16 @@
       <c r="H15">
         <v>9</v>
       </c>
-      <c r="M15" s="31">
+      <c r="M15" s="30">
         <v>8</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="30">
         <v>16</v>
       </c>
-      <c r="O15" s="32">
+      <c r="O15" s="31">
         <v>24</v>
       </c>
-      <c r="P15" s="30">
+      <c r="P15" s="29">
         <v>32</v>
       </c>
     </row>
@@ -1511,16 +1512,16 @@
       <c r="H16">
         <v>12</v>
       </c>
-      <c r="M16" s="28">
+      <c r="M16" s="27">
         <v>9</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="27">
         <v>18</v>
       </c>
-      <c r="O16" s="29">
+      <c r="O16" s="28">
         <v>27</v>
       </c>
-      <c r="P16" s="27">
+      <c r="P16" s="26">
         <v>36</v>
       </c>
     </row>
@@ -1540,16 +1541,16 @@
       <c r="H17">
         <v>15</v>
       </c>
-      <c r="M17" s="36">
+      <c r="M17" s="35">
         <v>10</v>
       </c>
-      <c r="N17" s="36">
+      <c r="N17" s="35">
         <v>20</v>
       </c>
-      <c r="O17" s="37">
+      <c r="O17" s="36">
         <v>30</v>
       </c>
-      <c r="P17" s="38">
+      <c r="P17" s="37">
         <v>40</v>
       </c>
     </row>

</xml_diff>